<commit_message>
edited spaces and headers in eDNA 01 and 02
</commit_message>
<xml_diff>
--- a/docs/eDNA/example_output/ASV_breakdown.xlsx
+++ b/docs/eDNA/example_output/ASV_breakdown.xlsx
@@ -1512,22 +1512,22 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>307c55294ffe3b8aa46fce358d55590e</t>
+          <t>c0a3f3ed23f04247d92740a9502f8b57</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>unassigned</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>unassigned</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>unassigned</t>
         </is>
       </c>
       <c r="E42">
@@ -1540,22 +1540,22 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>c0a3f3ed23f04247d92740a9502f8b57</t>
+          <t>307c55294ffe3b8aa46fce358d55590e</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E43">

</xml_diff>

<commit_message>
eDNA workflow with 03 and 04
</commit_message>
<xml_diff>
--- a/docs/eDNA/example_output/ASV_breakdown.xlsx
+++ b/docs/eDNA/example_output/ASV_breakdown.xlsx
@@ -1512,22 +1512,22 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>c0a3f3ed23f04247d92740a9502f8b57</t>
+          <t>307c55294ffe3b8aa46fce358d55590e</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E42">
@@ -1540,22 +1540,22 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>307c55294ffe3b8aa46fce358d55590e</t>
+          <t>c0a3f3ed23f04247d92740a9502f8b57</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>unassigned</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>unassigned</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>unassigned</t>
         </is>
       </c>
       <c r="E43">
@@ -1876,22 +1876,22 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>975b1dbdc7405f6e27bf63893e91e0ed</t>
+          <t>5e733a21f67e541f28ed4bf4fe025044</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Centropristis striata</t>
+          <t>unassigned</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Black sea bass</t>
+          <t>unassigned</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>unassigned</t>
         </is>
       </c>
       <c r="E55">
@@ -1904,22 +1904,22 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>5e733a21f67e541f28ed4bf4fe025044</t>
+          <t>975b1dbdc7405f6e27bf63893e91e0ed</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Centropristis striata</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Black sea bass</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E56">

</xml_diff>

<commit_message>
editing 02 for common name additions
</commit_message>
<xml_diff>
--- a/docs/eDNA/example_output/ASV_breakdown.xlsx
+++ b/docs/eDNA/example_output/ASV_breakdown.xlsx
@@ -1153,17 +1153,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E29">
@@ -1489,17 +1489,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E41">
@@ -1512,22 +1512,22 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>307c55294ffe3b8aa46fce358d55590e</t>
+          <t>c0a3f3ed23f04247d92740a9502f8b57</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E42">
@@ -1540,22 +1540,22 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>c0a3f3ed23f04247d92740a9502f8b57</t>
+          <t>307c55294ffe3b8aa46fce358d55590e</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E43">
@@ -1876,22 +1876,22 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>5e733a21f67e541f28ed4bf4fe025044</t>
+          <t>975b1dbdc7405f6e27bf63893e91e0ed</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Centropristis striata</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Black sea bass</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E55">
@@ -1904,22 +1904,22 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>975b1dbdc7405f6e27bf63893e91e0ed</t>
+          <t>5e733a21f67e541f28ed4bf4fe025044</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Centropristis striata</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Black sea bass</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E56">
@@ -2021,17 +2021,17 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E60">

</xml_diff>